<commit_message>
Update rocket engine input spreadsheet
Revised 'Inputs for Liquid Engine Rocket.xlsx' with updated data or parameters for liquid engine rocket calculations.
</commit_message>
<xml_diff>
--- a/Inputs for Liquid Engine Rocket.xlsx
+++ b/Inputs for Liquid Engine Rocket.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hamat\OneDrive\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hamat\OneDrive\Documents\GitHub\SRL-Taipan-Tank-Sizing-Model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1F4C3C25-3CDE-475D-AA08-7FCABC16BB0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A46478F-3A29-435F-9BA5-92480FEC7F59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14620" xr2:uid="{BFFCD3EE-9D90-47FE-B215-23123D0AB5C5}"/>
+    <workbookView xWindow="-90" yWindow="0" windowWidth="19380" windowHeight="14490" xr2:uid="{BFFCD3EE-9D90-47FE-B215-23123D0AB5C5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,9 +35,155 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="47">
+  <si>
+    <t>Inputs for Liquid Engine Rocket</t>
+  </si>
+  <si>
+    <t>Engine Preformance</t>
+  </si>
+  <si>
+    <t>Propellants &amp; Pressurant</t>
+  </si>
+  <si>
+    <t>Vehicle Geometry &amp; Materials</t>
+  </si>
+  <si>
+    <t>Design Margins &amp; Factors</t>
+  </si>
+  <si>
+    <t>Estimated Masses (Non-Calculated)</t>
+  </si>
+  <si>
+    <t>Design Constraints</t>
+  </si>
+  <si>
+    <t>Engine Thrust</t>
+  </si>
+  <si>
+    <t>f_thrust_n</t>
+  </si>
+  <si>
+    <t>Input</t>
+  </si>
+  <si>
+    <t>Variable Name</t>
+  </si>
+  <si>
+    <t>Unit</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>Specific Impulse</t>
+  </si>
+  <si>
+    <t>i_sp_s</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>t_burn_s</t>
+  </si>
+  <si>
+    <t>o_f_ratio</t>
+  </si>
+  <si>
+    <t>Total burn time</t>
+  </si>
+  <si>
+    <t>Oxidizer-to-Fuel mass ratio</t>
+  </si>
+  <si>
+    <t>unitless</t>
+  </si>
+  <si>
+    <t>ox_density_kgm3</t>
+  </si>
+  <si>
+    <t>fuel_density_kgm3</t>
+  </si>
+  <si>
+    <t>pressurant_molar_mass_kgmol</t>
+  </si>
+  <si>
+    <t>residual_fraction</t>
+  </si>
+  <si>
+    <t>Density of Liquid Oxygen</t>
+  </si>
+  <si>
+    <t>Density of Jet-A</t>
+  </si>
+  <si>
+    <t>Molar mass of Nitrogen (N2)</t>
+  </si>
+  <si>
+    <t>Percentage of fuel left over in tank after burnout</t>
+  </si>
+  <si>
+    <t>kg/m^3</t>
+  </si>
+  <si>
+    <t>kg/mol</t>
+  </si>
+  <si>
+    <t>p_op_ox_tank_pa</t>
+  </si>
+  <si>
+    <t>p_op_fuel_tank_pa</t>
+  </si>
+  <si>
+    <t>p_storage_pressurant_pa</t>
+  </si>
+  <si>
+    <t>ox_temp_k</t>
+  </si>
+  <si>
+    <t>fuel_temp_k</t>
+  </si>
+  <si>
+    <t>pressurant_temp_k</t>
+  </si>
+  <si>
+    <t>Operating pressure of LOX tank</t>
+  </si>
+  <si>
+    <t>Operating pressure of Fuel tank</t>
+  </si>
+  <si>
+    <t>The pressure the Nitrogen is stored in dedicated tank (MEOP)</t>
+  </si>
+  <si>
+    <t>Temperature of LOX in tank</t>
+  </si>
+  <si>
+    <t>Temperature of Jet-A in tank</t>
+  </si>
+  <si>
+    <t>Temperature of pressurant gas in its tank</t>
+  </si>
+  <si>
+    <t>Pa</t>
+  </si>
+  <si>
+    <t>K</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -45,16 +191,55 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="26"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="9" tint="-0.249977111117893"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -62,12 +247,80 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -402,14 +655,309 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7ABAC5D6-8C2E-46E8-B4A0-A363405B0DE5}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:AE21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="8.7265625" style="1"/>
+    <col min="2" max="2" width="23" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="8.7265625" style="1"/>
+    <col min="7" max="7" width="23.26953125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="51.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="33.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="8.7265625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:31" ht="32.5" x14ac:dyDescent="0.65">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="B3" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="7"/>
+      <c r="H3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="7"/>
+      <c r="M3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="N3" s="3"/>
+      <c r="O3" s="3"/>
+      <c r="P3" s="3"/>
+      <c r="R3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="S3" s="3"/>
+      <c r="T3" s="3"/>
+      <c r="U3" s="3"/>
+      <c r="W3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="X3" s="3"/>
+      <c r="Y3" s="3"/>
+      <c r="Z3" s="3"/>
+      <c r="AB3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="AC3" s="3"/>
+      <c r="AD3" s="3"/>
+      <c r="AE3" s="3"/>
+    </row>
+    <row r="4" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="B4" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="H4" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="I4" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="J4" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="K4" s="10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:31" ht="15" x14ac:dyDescent="0.4">
+      <c r="B5" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="H5" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I5" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="K5" s="4"/>
+    </row>
+    <row r="6" spans="1:31" ht="15" x14ac:dyDescent="0.4">
+      <c r="B6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="H6" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="I6" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="K6" s="4"/>
+    </row>
+    <row r="7" spans="1:31" ht="15" x14ac:dyDescent="0.4">
+      <c r="B7" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="H7" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="I7" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="K7" s="4"/>
+    </row>
+    <row r="8" spans="1:31" ht="15" x14ac:dyDescent="0.4">
+      <c r="B8" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="H8" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="I8" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="J8" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="K8" s="4"/>
+    </row>
+    <row r="9" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="8"/>
+    </row>
+    <row r="10" spans="1:31" ht="15" x14ac:dyDescent="0.4">
+      <c r="H10" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="I10" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="J10" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="K10" s="4"/>
+    </row>
+    <row r="11" spans="1:31" ht="15" x14ac:dyDescent="0.4">
+      <c r="H11" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="I11" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="J11" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="K11" s="4"/>
+    </row>
+    <row r="12" spans="1:31" ht="15" x14ac:dyDescent="0.4">
+      <c r="H12" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="I12" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="J12" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="K12" s="4"/>
+    </row>
+    <row r="13" spans="1:31" ht="15" x14ac:dyDescent="0.4">
+      <c r="H13" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="I13" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="J13" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="K13" s="4"/>
+    </row>
+    <row r="14" spans="1:31" ht="15" x14ac:dyDescent="0.4">
+      <c r="H14" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="I14" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="J14" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="K14" s="4"/>
+    </row>
+    <row r="15" spans="1:31" ht="15" x14ac:dyDescent="0.4">
+      <c r="H15" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="I15" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="J15" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="K15" s="4"/>
+    </row>
+    <row r="16" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="H16" s="4"/>
+      <c r="I16" s="4"/>
+      <c r="J16" s="4"/>
+      <c r="K16" s="4"/>
+    </row>
+    <row r="17" spans="8:11" x14ac:dyDescent="0.3">
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="4"/>
+      <c r="K17" s="4"/>
+    </row>
+    <row r="18" spans="8:11" x14ac:dyDescent="0.3">
+      <c r="H18" s="4"/>
+      <c r="I18" s="4"/>
+      <c r="J18" s="4"/>
+      <c r="K18" s="4"/>
+    </row>
+    <row r="19" spans="8:11" x14ac:dyDescent="0.3">
+      <c r="H19" s="4"/>
+      <c r="I19" s="4"/>
+      <c r="J19" s="4"/>
+      <c r="K19" s="4"/>
+    </row>
+    <row r="20" spans="8:11" x14ac:dyDescent="0.3">
+      <c r="H20" s="4"/>
+      <c r="I20" s="4"/>
+      <c r="J20" s="4"/>
+      <c r="K20" s="4"/>
+    </row>
+    <row r="21" spans="8:11" x14ac:dyDescent="0.3">
+      <c r="H21" s="4"/>
+      <c r="I21" s="4"/>
+      <c r="J21" s="4"/>
+      <c r="K21" s="4"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="H3:K3"/>
+    <mergeCell ref="B3:F3"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update Inputs for Liquid Engine Rocket.xlsx
</commit_message>
<xml_diff>
--- a/Inputs for Liquid Engine Rocket.xlsx
+++ b/Inputs for Liquid Engine Rocket.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hamat\OneDrive\Documents\GitHub\SRL-Taipan-Tank-Sizing-Model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A46478F-3A29-435F-9BA5-92480FEC7F59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18DA98DC-2A45-44DF-A267-2E0B7BAD8770}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="0" windowWidth="19380" windowHeight="14490" xr2:uid="{BFFCD3EE-9D90-47FE-B215-23123D0AB5C5}"/>
+    <workbookView xWindow="20" yWindow="0" windowWidth="25580" windowHeight="14380" xr2:uid="{BFFCD3EE-9D90-47FE-B215-23123D0AB5C5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -309,6 +309,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -318,9 +321,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -658,7 +658,7 @@
   <dimension ref="A1:AE21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -679,19 +679,19 @@
       </c>
     </row>
     <row r="3" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="7"/>
-      <c r="H3" s="5" t="s">
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="10"/>
+      <c r="H3" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="7"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="10"/>
       <c r="M3" s="3" t="s">
         <v>3</v>
       </c>
@@ -718,31 +718,31 @@
       <c r="AE3" s="3"/>
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="E4" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="10" t="s">
+      <c r="F4" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="H4" s="10" t="s">
+      <c r="H4" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="I4" s="10" t="s">
+      <c r="I4" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="J4" s="10" t="s">
+      <c r="J4" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="K4" s="10" t="s">
+      <c r="K4" s="7" t="s">
         <v>12</v>
       </c>
     </row>
@@ -750,7 +750,7 @@
       <c r="B5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="6" t="s">
         <v>8</v>
       </c>
       <c r="D5" s="4" t="s">
@@ -761,7 +761,7 @@
       <c r="H5" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="I5" s="9" t="s">
+      <c r="I5" s="6" t="s">
         <v>22</v>
       </c>
       <c r="J5" s="4" t="s">
@@ -773,7 +773,7 @@
       <c r="B6" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="6" t="s">
         <v>15</v>
       </c>
       <c r="D6" s="4" t="s">
@@ -784,7 +784,7 @@
       <c r="H6" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="I6" s="9" t="s">
+      <c r="I6" s="6" t="s">
         <v>23</v>
       </c>
       <c r="J6" s="4" t="s">
@@ -796,7 +796,7 @@
       <c r="B7" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="6" t="s">
         <v>17</v>
       </c>
       <c r="D7" s="4" t="s">
@@ -807,7 +807,7 @@
       <c r="H7" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="I7" s="9" t="s">
+      <c r="I7" s="6" t="s">
         <v>24</v>
       </c>
       <c r="J7" s="4" t="s">
@@ -819,7 +819,7 @@
       <c r="B8" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="6" t="s">
         <v>18</v>
       </c>
       <c r="D8" s="4" t="s">
@@ -830,7 +830,7 @@
       <c r="H8" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="I8" s="9" t="s">
+      <c r="I8" s="6" t="s">
         <v>25</v>
       </c>
       <c r="J8" s="4" t="s">
@@ -839,16 +839,16 @@
       <c r="K8" s="4"/>
     </row>
     <row r="9" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="H9" s="8"/>
-      <c r="I9" s="8"/>
-      <c r="J9" s="8"/>
-      <c r="K9" s="8"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="5"/>
     </row>
     <row r="10" spans="1:31" ht="15" x14ac:dyDescent="0.4">
       <c r="H10" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="I10" s="9" t="s">
+      <c r="I10" s="6" t="s">
         <v>32</v>
       </c>
       <c r="J10" s="4" t="s">
@@ -860,7 +860,7 @@
       <c r="H11" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="I11" s="9" t="s">
+      <c r="I11" s="6" t="s">
         <v>33</v>
       </c>
       <c r="J11" s="4" t="s">
@@ -872,7 +872,7 @@
       <c r="H12" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="I12" s="9" t="s">
+      <c r="I12" s="6" t="s">
         <v>34</v>
       </c>
       <c r="J12" s="4" t="s">
@@ -884,7 +884,7 @@
       <c r="H13" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="I13" s="9" t="s">
+      <c r="I13" s="6" t="s">
         <v>35</v>
       </c>
       <c r="J13" s="4" t="s">
@@ -896,7 +896,7 @@
       <c r="H14" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="I14" s="9" t="s">
+      <c r="I14" s="6" t="s">
         <v>36</v>
       </c>
       <c r="J14" s="4" t="s">
@@ -908,7 +908,7 @@
       <c r="H15" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="I15" s="9" t="s">
+      <c r="I15" s="6" t="s">
         <v>37</v>
       </c>
       <c r="J15" s="4" t="s">

</xml_diff>